<commit_message>
countries - cities - districts component
</commit_message>
<xml_diff>
--- a/GP1_Planlama.xlsx
+++ b/GP1_Planlama.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED5774B-7F89-42E0-89BD-43F786C5440A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13410"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,7 +194,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,20 +455,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Giriş" xfId="3" builtinId="20"/>
+    <cellStyle name="İyi" xfId="1" builtinId="26"/>
+    <cellStyle name="Kötü" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -745,12 +746,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3"/>
+      <selection pane="topRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,46 +762,46 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14" t="s">
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14" t="s">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14" t="s">
+      <c r="S1" s="15"/>
+      <c r="T1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="15"/>
+      <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -874,10 +875,10 @@
       <c r="D3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -932,7 +933,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -997,7 +998,7 @@
       <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1062,7 +1063,7 @@
       <c r="C6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1127,7 +1128,7 @@
       <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1192,7 +1193,7 @@
       <c r="C8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1251,13 +1252,13 @@
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E9" s="10" t="s">

</xml_diff>